<commit_message>
minor updates to main
</commit_message>
<xml_diff>
--- a/data-fix/all_features_in.xlsx
+++ b/data-fix/all_features_in.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\phosphine-ligands\data-fix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD11EDF1-263D-4228-B91A-8345A85F5BD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B17F5A-E508-4DE4-B355-EFD6A9D09BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5185,7 +5185,7 @@
   <dimension ref="A1:BO100"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
exploring non linear PC1 fitting
</commit_message>
<xml_diff>
--- a/data-fix/all_features_in.xlsx
+++ b/data-fix/all_features_in.xlsx
@@ -8,182 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jwb1j\OneDrive\Documents\GitHub\phosphine-ligands\data-fix\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B17F5A-E508-4DE4-B355-EFD6A9D09BBC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF580FA7-B794-4CDC-A4C4-8FFDE671AE80}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="26301" windowHeight="14427" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-26192" yWindow="-109" windowWidth="26301" windowHeight="14889" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Sheet1!$AC$108</definedName>
-    <definedName name="_xlchart.v1.100" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.101" hidden="1">Sheet1!$G$108</definedName>
-    <definedName name="_xlchart.v1.102" hidden="1">Sheet1!$G$108:$G$109</definedName>
-    <definedName name="_xlchart.v1.103" hidden="1">Sheet1!$G$58:$G$109</definedName>
-    <definedName name="_xlchart.v1.104" hidden="1">Sheet1!$H$1</definedName>
-    <definedName name="_xlchart.v1.105" hidden="1">Sheet1!$H$108</definedName>
-    <definedName name="_xlchart.v1.106" hidden="1">Sheet1!$H$108:$H$109</definedName>
-    <definedName name="_xlchart.v1.107" hidden="1">Sheet1!$H$58:$H$109</definedName>
-    <definedName name="_xlchart.v1.108" hidden="1">Sheet1!$I$1</definedName>
-    <definedName name="_xlchart.v1.109" hidden="1">Sheet1!$I$108</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Sheet1!$AD$1</definedName>
-    <definedName name="_xlchart.v1.110" hidden="1">Sheet1!$J$1</definedName>
-    <definedName name="_xlchart.v1.111" hidden="1">Sheet1!$J$108</definedName>
-    <definedName name="_xlchart.v1.112" hidden="1">Sheet1!$K$1</definedName>
-    <definedName name="_xlchart.v1.113" hidden="1">Sheet1!$K$108</definedName>
-    <definedName name="_xlchart.v1.114" hidden="1">Sheet1!$L$1</definedName>
-    <definedName name="_xlchart.v1.115" hidden="1">Sheet1!$L$108</definedName>
-    <definedName name="_xlchart.v1.116" hidden="1">Sheet1!$M$1</definedName>
-    <definedName name="_xlchart.v1.117" hidden="1">Sheet1!$M$108</definedName>
-    <definedName name="_xlchart.v1.118" hidden="1">Sheet1!$N$1</definedName>
-    <definedName name="_xlchart.v1.119" hidden="1">Sheet1!$N$108</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Sheet1!$AD$108</definedName>
-    <definedName name="_xlchart.v1.120" hidden="1">Sheet1!$O$1</definedName>
-    <definedName name="_xlchart.v1.121" hidden="1">Sheet1!$O$108</definedName>
-    <definedName name="_xlchart.v1.122" hidden="1">Sheet1!$P$1</definedName>
-    <definedName name="_xlchart.v1.123" hidden="1">Sheet1!$P$108</definedName>
-    <definedName name="_xlchart.v1.124" hidden="1">Sheet1!$Q$1</definedName>
-    <definedName name="_xlchart.v1.125" hidden="1">Sheet1!$Q$108</definedName>
-    <definedName name="_xlchart.v1.126" hidden="1">Sheet1!$R$1</definedName>
-    <definedName name="_xlchart.v1.127" hidden="1">Sheet1!$R$108</definedName>
-    <definedName name="_xlchart.v1.128" hidden="1">Sheet1!$S$1</definedName>
-    <definedName name="_xlchart.v1.129" hidden="1">Sheet1!$S$108</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Sheet1!$AE$1</definedName>
-    <definedName name="_xlchart.v1.130" hidden="1">Sheet1!$T$1</definedName>
-    <definedName name="_xlchart.v1.131" hidden="1">Sheet1!$T$108</definedName>
-    <definedName name="_xlchart.v1.132" hidden="1">Sheet1!$U$1</definedName>
-    <definedName name="_xlchart.v1.133" hidden="1">Sheet1!$U$108</definedName>
-    <definedName name="_xlchart.v1.134" hidden="1">Sheet1!$V$1</definedName>
-    <definedName name="_xlchart.v1.135" hidden="1">Sheet1!$V$108</definedName>
-    <definedName name="_xlchart.v1.136" hidden="1">Sheet1!$W$1</definedName>
-    <definedName name="_xlchart.v1.137" hidden="1">Sheet1!$W$108</definedName>
-    <definedName name="_xlchart.v1.138" hidden="1">Sheet1!$X$1</definedName>
-    <definedName name="_xlchart.v1.139" hidden="1">Sheet1!$X$108</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Sheet1!$AE$108</definedName>
-    <definedName name="_xlchart.v1.140" hidden="1">Sheet1!$Y$1</definedName>
-    <definedName name="_xlchart.v1.141" hidden="1">Sheet1!$Y$108</definedName>
-    <definedName name="_xlchart.v1.142" hidden="1">Sheet1!$Z$1</definedName>
-    <definedName name="_xlchart.v1.143" hidden="1">Sheet1!$Z$108</definedName>
-    <definedName name="_xlchart.v1.144" hidden="1">Sheet2!$A$1</definedName>
-    <definedName name="_xlchart.v1.145" hidden="1">Sheet2!$A$2:$A$2</definedName>
-    <definedName name="_xlchart.v1.146" hidden="1">Sheet2!$A$2:$A$60</definedName>
-    <definedName name="_xlchart.v1.147" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.148" hidden="1">Sheet1!$G$2:$G$93</definedName>
-    <definedName name="_xlchart.v1.149" hidden="1">Sheet2!$A$1</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Sheet1!$AF$1</definedName>
-    <definedName name="_xlchart.v1.150" hidden="1">Sheet2!$A$2:$A$60</definedName>
-    <definedName name="_xlchart.v1.151" hidden="1">Sheet2!$A$1</definedName>
-    <definedName name="_xlchart.v1.152" hidden="1">Sheet2!$A$2:$A$60</definedName>
-    <definedName name="_xlchart.v1.153" hidden="1">Sheet2!$B$1</definedName>
-    <definedName name="_xlchart.v1.154" hidden="1">Sheet2!$B$2:$B$60</definedName>
-    <definedName name="_xlchart.v1.155" hidden="1">Sheet2!$A$1</definedName>
-    <definedName name="_xlchart.v1.156" hidden="1">Sheet2!$A$2:$A$60</definedName>
-    <definedName name="_xlchart.v1.157" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.158" hidden="1">Sheet1!$G$2:$G$93</definedName>
-    <definedName name="_xlchart.v1.159" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Sheet1!$AF$108</definedName>
-    <definedName name="_xlchart.v1.160" hidden="1">Sheet1!$F$2:$F$93</definedName>
-    <definedName name="_xlchart.v1.161" hidden="1">Sheet1!$G$1</definedName>
-    <definedName name="_xlchart.v1.162" hidden="1">Sheet1!$G$2:$G$93</definedName>
-    <definedName name="_xlchart.v1.163" hidden="1">Sheet2!$A$1</definedName>
-    <definedName name="_xlchart.v1.164" hidden="1">Sheet2!$A$2:$A$60</definedName>
-    <definedName name="_xlchart.v1.165" hidden="1">Sheet2!$B$1</definedName>
-    <definedName name="_xlchart.v1.166" hidden="1">Sheet2!$B$2:$B$60</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Sheet1!$AG$1</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Sheet1!$AG$108</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Sheet1!$AH$1</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Sheet1!$D$2:$D$94</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Sheet1!$AH$108</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Sheet1!$AI$1</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Sheet1!$AI$108</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Sheet1!$AJ$1</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Sheet1!$AJ$108</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Sheet1!$AK$1</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Sheet1!$AK$108</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Sheet1!$AL$1</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Sheet1!$AL$108</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Sheet1!$AM$1</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Sheet1!#REF!</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Sheet1!$AM$108</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Sheet1!$AN$1</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Sheet1!$AN$108</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Sheet1!$AO$1</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Sheet1!$AO$108</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Sheet1!$AP$1</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Sheet1!$AP$108</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Sheet1!$AQ$1</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Sheet1!$AQ$108</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Sheet1!$AR$1</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Sheet1!$A$108</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Sheet1!$AR$108</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Sheet1!$AS$1</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Sheet1!$AS$108</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Sheet1!$AT$1</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Sheet1!$AT$108</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Sheet1!$AU$1</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Sheet1!$AU$108</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Sheet1!$AV$1</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Sheet1!$AV$108</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Sheet1!$AW$1</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Sheet1!$AA$1</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Sheet1!$AW$108</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Sheet1!$AX$1</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Sheet1!$AX$108</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Sheet1!$AY$1</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Sheet1!$AY$108</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Sheet1!$AZ$1</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Sheet1!$AZ$108</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Sheet1!$B$1</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Sheet1!$BA$1</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Sheet1!$BA$108</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$AA$108</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Sheet1!$BB$1</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Sheet1!$BB$108</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Sheet1!$BC$1</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Sheet1!$BC$108</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Sheet1!$BD$1</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Sheet1!$BD$108</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Sheet1!$BE$1</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Sheet1!$BE$108</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">Sheet1!$BF$1</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">Sheet1!$BF$108</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$AB$1</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">Sheet1!$BG$1</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">Sheet1!$BG$108</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">Sheet1!$BH$1</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">Sheet1!$BH$108</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">Sheet1!$BI$1</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">Sheet1!$BI$108</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">Sheet1!$BJ$1</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">Sheet1!$BJ$108</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">Sheet1!$BK$1</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">Sheet1!$BK$108</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$AB$108</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">Sheet1!$BL$1</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">Sheet1!$BL$108</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">Sheet1!$BM$1</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">Sheet1!$BM$108</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">Sheet1!$C$1</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">Sheet1!$C$108</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">Sheet1!$C$108:$C$109</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">Sheet1!$D$1</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">Sheet1!$D$108</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">Sheet1!$D$108:$D$109</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$AC$1</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">Sheet1!$D$2:$D$94</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">Sheet1!$E$1</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">Sheet1!$E$108</definedName>
-    <definedName name="_xlchart.v1.93" hidden="1">Sheet1!$E$108:$E$109</definedName>
-    <definedName name="_xlchart.v1.94" hidden="1">Sheet1!$E$58:$E$109</definedName>
-    <definedName name="_xlchart.v1.95" hidden="1">Sheet1!$E$58:$E$150</definedName>
-    <definedName name="_xlchart.v1.96" hidden="1">Sheet1!$F$1</definedName>
-    <definedName name="_xlchart.v1.97" hidden="1">Sheet1!$F$108</definedName>
-    <definedName name="_xlchart.v1.98" hidden="1">Sheet1!$F$108:$F$109</definedName>
-    <definedName name="_xlchart.v1.99" hidden="1">Sheet1!$F$58:$F$109</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Sheet1!$D$1</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Sheet1!$D$2:$D$94</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Sheet2!$B$1</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Sheet2!$B$2:$B$60</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Sheet2!$A$1</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Sheet2!$A$2:$A$60</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Sheet1!$F$1</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Sheet1!$F$2:$F$93</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$G$1</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$G$2:$G$93</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -895,7 +738,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -943,7 +786,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-ED6E-4734-91CE-2DA332850DF6}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.0</cx:f>
               <cx:v>nbmi</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1070,7 +913,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.156</cx:f>
+        <cx:f>_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1118,7 +961,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{000000C0-5167-44DC-8C6C-53A28732D6D7}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.155</cx:f>
+              <cx:f>_xlchart.v1.4</cx:f>
               <cx:v>1m2 train</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1245,7 +1088,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.158</cx:f>
+        <cx:f>_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1293,7 +1136,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-B610-432D-AA7F-54070C1851BD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.157</cx:f>
+              <cx:f>_xlchart.v1.8</cx:f>
               <cx:v>1m2</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1421,7 +1264,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.154</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1469,7 +1312,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{F7E19050-310E-4AD5-890A-E8D1BD993146}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.153</cx:f>
+              <cx:f>_xlchart.v1.2</cx:f>
               <cx:v>bmi train</cx:v>
             </cx:txData>
           </cx:tx>
@@ -1596,7 +1439,7 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.160</cx:f>
+        <cx:f>_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1656,7 +1499,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{00000000-B610-432D-AA7F-54070C1851BD}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.159</cx:f>
+              <cx:f>_xlchart.v1.6</cx:f>
               <cx:v>bmi</cx:v>
             </cx:txData>
           </cx:tx>
@@ -4568,7 +4411,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="4464170" y="638352"/>
+              <a:off x="7155611" y="638352"/>
               <a:ext cx="4572000" cy="2562045"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -5184,9 +5027,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO100"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A71" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A61" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14:H94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -24500,8 +24343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5D6CFF9-DE61-4B91-994F-A3819997C4A3}">
   <dimension ref="A1:I60"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" topLeftCell="B64" workbookViewId="0">
+      <selection activeCell="Y82" sqref="Y2:Y82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -25167,6 +25010,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="Y2:Y82">
+    <sortCondition ref="Y2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>